<commit_message>
Preparando para testar timeOutAYC
</commit_message>
<xml_diff>
--- a/docs/Avaliação dos resultados - T1.xlsx
+++ b/docs/Avaliação dos resultados - T1.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Número de mensagens trocadas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>step</t>
   </si>
@@ -30,6 +30,30 @@
   <si>
     <t>Rounds necessários para convergência</t>
   </si>
+  <si>
+    <t>AYCoord</t>
+  </si>
+  <si>
+    <t>AY_Answer</t>
+  </si>
+  <si>
+    <t>Invitation</t>
+  </si>
+  <si>
+    <t>Accept</t>
+  </si>
+  <si>
+    <t>Accept_answer</t>
+  </si>
+  <si>
+    <t>Ready</t>
+  </si>
+  <si>
+    <t>Ready_answer</t>
+  </si>
+  <si>
+    <t>Total abstrato</t>
+  </si>
 </sst>
 </file>
 
@@ -37,7 +61,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -520,8 +544,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -671,31 +695,31 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>133</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>525</c:v>
+                  <c:v>555</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2077</c:v>
+                  <c:v>2139</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8253</c:v>
+                  <c:v>8379</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32893</c:v>
+                  <c:v>33147</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>131325</c:v>
+                  <c:v>131835</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>524797</c:v>
+                  <c:v>525819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -712,11 +736,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="138138368"/>
-        <c:axId val="138139904"/>
+        <c:axId val="116078464"/>
+        <c:axId val="116080000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="138138368"/>
+        <c:axId val="116078464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -726,7 +750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138139904"/>
+        <c:crossAx val="116080000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -734,7 +758,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138139904"/>
+        <c:axId val="116080000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,7 +769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138138368"/>
+        <c:crossAx val="116078464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -881,31 +905,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -922,11 +946,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="54699520"/>
-        <c:axId val="54701056"/>
+        <c:axId val="116104576"/>
+        <c:axId val="116122752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54699520"/>
+        <c:axId val="116104576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,7 +960,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54701056"/>
+        <c:crossAx val="116122752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -944,7 +968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54701056"/>
+        <c:axId val="116122752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,7 +979,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54699520"/>
+        <c:crossAx val="116104576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1012,15 +1036,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1329,10 +1353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,9 +1364,13 @@
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" customWidth="1"/>
     <col min="5" max="5" width="36.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1358,8 +1386,32 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>64</v>
       </c>
@@ -1370,14 +1422,49 @@
         <v>2</v>
       </c>
       <c r="D2" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2">
-        <v>63</v>
-      </c>
-      <c r="G2" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="G2" s="2">
+        <f>C2*C2-C2</f>
+        <v>2</v>
+      </c>
+      <c r="H2" s="2">
+        <f>C2*C2-C2</f>
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <f>C2-1</f>
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f>C2-1</f>
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>C2-1</f>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f>C2-1</f>
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <f>C2-1</f>
+        <v>1</v>
+      </c>
+      <c r="N2" s="2">
+        <f>SUM(G2:M2)</f>
+        <v>9</v>
+      </c>
+      <c r="O2">
+        <f>2* (POWER(C2,2)) + 3*C2 - 5</f>
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>164</v>
       </c>
@@ -1388,14 +1475,49 @@
         <v>4</v>
       </c>
       <c r="D3" s="1">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E3">
-        <v>63</v>
-      </c>
-      <c r="G3" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="G3" s="2">
+        <f>C3*C3-C3</f>
+        <v>12</v>
+      </c>
+      <c r="H3" s="2">
+        <f>C3*C3-C3</f>
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <f>C3-1</f>
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <f>C3-1</f>
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <f>C3-1</f>
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <f>C3-1</f>
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <f>C3-1</f>
+        <v>3</v>
+      </c>
+      <c r="N3" s="2">
+        <f>SUM(G3:M3)</f>
+        <v>39</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O10" si="0">2* (POWER(C3,2)) + 3*C3 - 5</f>
+        <v>39</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>314</v>
       </c>
@@ -1406,14 +1528,49 @@
         <v>8</v>
       </c>
       <c r="D4" s="1">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="E4">
-        <v>63</v>
-      </c>
-      <c r="G4" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G10" si="1">C4*C4-C4</f>
+        <v>56</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H10" si="2">C4*C4-C4</f>
+        <v>56</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I10" si="3">C4-1</f>
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J10" si="4">C4-1</f>
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K10" si="5">C4-1</f>
+        <v>7</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L10" si="6">C4-1</f>
+        <v>7</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M10" si="7">C4-1</f>
+        <v>7</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N10" si="8">SUM(G4:M4)</f>
+        <v>147</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>464</v>
       </c>
@@ -1424,14 +1581,49 @@
         <v>16</v>
       </c>
       <c r="D5" s="1">
-        <v>525</v>
+        <v>555</v>
       </c>
       <c r="E5">
-        <v>63</v>
-      </c>
-      <c r="G5" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="8"/>
+        <v>555</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>555</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>614</v>
       </c>
@@ -1442,14 +1634,49 @@
         <v>32</v>
       </c>
       <c r="D6" s="1">
-        <v>2077</v>
+        <v>2139</v>
       </c>
       <c r="E6">
-        <v>63</v>
-      </c>
-      <c r="G6" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
+        <v>992</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="2"/>
+        <v>992</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="7"/>
+        <v>31</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="8"/>
+        <v>2139</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>2139</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>714</v>
       </c>
@@ -1460,14 +1687,49 @@
         <v>64</v>
       </c>
       <c r="D7" s="1">
-        <v>8253</v>
+        <v>8379</v>
       </c>
       <c r="E7">
+        <v>66</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>4032</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="2"/>
+        <v>4032</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="5"/>
+        <v>63</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="6"/>
+        <v>63</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="7"/>
+        <v>63</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="8"/>
+        <v>8379</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>8379</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>864</v>
       </c>
@@ -1478,14 +1740,49 @@
         <v>128</v>
       </c>
       <c r="D8" s="1">
-        <v>32893</v>
+        <v>33147</v>
       </c>
       <c r="E8">
-        <v>63</v>
-      </c>
-      <c r="G8" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>16256</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="2"/>
+        <v>16256</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>127</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="5"/>
+        <v>127</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="6"/>
+        <v>127</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="7"/>
+        <v>127</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="8"/>
+        <v>33147</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>33147</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>964</v>
       </c>
@@ -1496,14 +1793,49 @@
         <v>256</v>
       </c>
       <c r="D9" s="1">
-        <v>131325</v>
+        <v>131835</v>
       </c>
       <c r="E9">
-        <v>63</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>65280</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="2"/>
+        <v>65280</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>255</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="5"/>
+        <v>255</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="6"/>
+        <v>255</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="8"/>
+        <v>131835</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>131835</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1214</v>
       </c>
@@ -1514,12 +1846,47 @@
         <v>512</v>
       </c>
       <c r="D10" s="1">
-        <v>524797</v>
+        <v>525819</v>
       </c>
       <c r="E10">
-        <v>63</v>
-      </c>
-      <c r="G10" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>261632</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="2"/>
+        <v>261632</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>511</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>511</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="5"/>
+        <v>511</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="6"/>
+        <v>511</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="7"/>
+        <v>511</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="8"/>
+        <v>525819</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>525819</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Primeira bateria de testes para relatório
</commit_message>
<xml_diff>
--- a/docs/Avaliação dos resultados - T1.xlsx
+++ b/docs/Avaliação dos resultados - T1.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Número de mensagens trocadas" sheetId="1" r:id="rId1"/>
+    <sheet name="Instabilidade" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>step</t>
   </si>
@@ -53,6 +57,18 @@
   </si>
   <si>
     <t>Total abstrato</t>
+  </si>
+  <si>
+    <t>qtdNosInstaveis</t>
+  </si>
+  <si>
+    <t>5N - 0.025</t>
+  </si>
+  <si>
+    <t>10N - 0.025</t>
+  </si>
+  <si>
+    <t>5N - 0.08</t>
   </si>
 </sst>
 </file>
@@ -736,11 +752,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116078464"/>
-        <c:axId val="116080000"/>
+        <c:axId val="69788032"/>
+        <c:axId val="69789568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116078464"/>
+        <c:axId val="69788032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -750,7 +766,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116080000"/>
+        <c:crossAx val="69789568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -758,7 +774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116080000"/>
+        <c:axId val="69789568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -769,7 +785,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116078464"/>
+        <c:crossAx val="69788032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -847,7 +863,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -946,11 +961,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116104576"/>
-        <c:axId val="116122752"/>
+        <c:axId val="69810048"/>
+        <c:axId val="69811584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116104576"/>
+        <c:axId val="69810048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,7 +975,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116122752"/>
+        <c:crossAx val="69811584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -968,7 +983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116122752"/>
+        <c:axId val="69811584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,13 +994,1984 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116104576"/>
+        <c:crossAx val="69810048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>5 nós - erro 0.25</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Instabilidade!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4900</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5100</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5200</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5300</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5600</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5700</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5800</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5900</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6100</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6300</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6700</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6900</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7100</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7200</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7300</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7400</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7600</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7700</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7900</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8100</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8200</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8300</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8400</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8600</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8700</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8800</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8900</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9100</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9200</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9300</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9400</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9600</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9700</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9800</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9900</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]0_25-05-2015-at-12-24-36-391-AM'!$C$2:$C$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>5 nós - erro 0.08</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Instabilidade!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4900</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5100</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5200</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5300</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5600</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5700</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5800</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5900</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6100</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6300</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6700</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6900</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7100</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7200</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7300</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7400</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7600</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7700</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7900</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8100</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8200</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8300</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8400</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8600</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8700</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8800</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8900</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9100</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9200</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9300</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9400</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9600</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9700</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9800</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9900</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Instabilidade!$E$2:$E$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>10 nós - erro 0.025</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Instabilidade!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4900</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5100</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5200</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5300</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5600</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5700</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5800</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5900</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6100</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6300</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6700</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6900</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7100</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7200</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7300</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7400</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7600</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7700</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7900</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8100</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8200</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8300</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8400</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8600</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8700</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8800</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8900</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9100</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9200</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9300</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9400</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9600</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9700</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9800</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9900</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Instabilidade!$D$2:$D$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="69593344"/>
+        <c:axId val="69763072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="69593344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69763072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69763072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69593344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -1064,6 +3050,857 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="0_25-05-2015-at-12-24-36-391-AM"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2">
+            <v>100</v>
+          </cell>
+          <cell r="C2">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>200</v>
+          </cell>
+          <cell r="C3">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>300</v>
+          </cell>
+          <cell r="C4">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>400</v>
+          </cell>
+          <cell r="C5">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>500</v>
+          </cell>
+          <cell r="C6">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>600</v>
+          </cell>
+          <cell r="C7">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>700</v>
+          </cell>
+          <cell r="C8">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>800</v>
+          </cell>
+          <cell r="C9">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>900</v>
+          </cell>
+          <cell r="C10">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>1000</v>
+          </cell>
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>1100</v>
+          </cell>
+          <cell r="C12">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>1200</v>
+          </cell>
+          <cell r="C13">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>1300</v>
+          </cell>
+          <cell r="C14">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>1400</v>
+          </cell>
+          <cell r="C15">
+            <v>20</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>1500</v>
+          </cell>
+          <cell r="C16">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>1600</v>
+          </cell>
+          <cell r="C17">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>1700</v>
+          </cell>
+          <cell r="C18">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>1800</v>
+          </cell>
+          <cell r="C19">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>1900</v>
+          </cell>
+          <cell r="C20">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>2000</v>
+          </cell>
+          <cell r="C21">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>2100</v>
+          </cell>
+          <cell r="C22">
+            <v>75</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>2200</v>
+          </cell>
+          <cell r="C23">
+            <v>20</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>2300</v>
+          </cell>
+          <cell r="C24">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>2400</v>
+          </cell>
+          <cell r="C25">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>2500</v>
+          </cell>
+          <cell r="C26">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>2600</v>
+          </cell>
+          <cell r="C27">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>2700</v>
+          </cell>
+          <cell r="C28">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>2800</v>
+          </cell>
+          <cell r="C29">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>2900</v>
+          </cell>
+          <cell r="C30">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>3000</v>
+          </cell>
+          <cell r="C31">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>3100</v>
+          </cell>
+          <cell r="C32">
+            <v>75</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>3200</v>
+          </cell>
+          <cell r="C33">
+            <v>20</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>3300</v>
+          </cell>
+          <cell r="C34">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>3400</v>
+          </cell>
+          <cell r="C35">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>3500</v>
+          </cell>
+          <cell r="C36">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>3600</v>
+          </cell>
+          <cell r="C37">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>3700</v>
+          </cell>
+          <cell r="C38">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>3800</v>
+          </cell>
+          <cell r="C39">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>3900</v>
+          </cell>
+          <cell r="C40">
+            <v>70</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>4000</v>
+          </cell>
+          <cell r="C41">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>4100</v>
+          </cell>
+          <cell r="C42">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>4200</v>
+          </cell>
+          <cell r="C43">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>4300</v>
+          </cell>
+          <cell r="C44">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>4400</v>
+          </cell>
+          <cell r="C45">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>4500</v>
+          </cell>
+          <cell r="C46">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>4600</v>
+          </cell>
+          <cell r="C47">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>4700</v>
+          </cell>
+          <cell r="C48">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>4800</v>
+          </cell>
+          <cell r="C49">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>4900</v>
+          </cell>
+          <cell r="C50">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>5000</v>
+          </cell>
+          <cell r="C51">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52">
+            <v>5100</v>
+          </cell>
+          <cell r="C52">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53">
+            <v>5200</v>
+          </cell>
+          <cell r="C53">
+            <v>70</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54">
+            <v>5300</v>
+          </cell>
+          <cell r="C54">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55">
+            <v>5400</v>
+          </cell>
+          <cell r="C55">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56">
+            <v>5500</v>
+          </cell>
+          <cell r="C56">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57">
+            <v>5600</v>
+          </cell>
+          <cell r="C57">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58">
+            <v>5700</v>
+          </cell>
+          <cell r="C58">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59">
+            <v>5800</v>
+          </cell>
+          <cell r="C59">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60">
+            <v>5900</v>
+          </cell>
+          <cell r="C60">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61">
+            <v>6000</v>
+          </cell>
+          <cell r="C61">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62">
+            <v>6100</v>
+          </cell>
+          <cell r="C62">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63">
+            <v>6200</v>
+          </cell>
+          <cell r="C63">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64">
+            <v>6300</v>
+          </cell>
+          <cell r="C64">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65">
+            <v>6400</v>
+          </cell>
+          <cell r="C65">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66">
+            <v>6500</v>
+          </cell>
+          <cell r="C66">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67">
+            <v>6600</v>
+          </cell>
+          <cell r="C67">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68">
+            <v>6700</v>
+          </cell>
+          <cell r="C68">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69">
+            <v>6800</v>
+          </cell>
+          <cell r="C69">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70">
+            <v>6900</v>
+          </cell>
+          <cell r="C70">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71">
+            <v>7000</v>
+          </cell>
+          <cell r="C71">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72">
+            <v>7100</v>
+          </cell>
+          <cell r="C72">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73">
+            <v>7200</v>
+          </cell>
+          <cell r="C73">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74">
+            <v>7300</v>
+          </cell>
+          <cell r="C74">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75">
+            <v>7400</v>
+          </cell>
+          <cell r="C75">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76">
+            <v>7500</v>
+          </cell>
+          <cell r="C76">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77">
+            <v>7600</v>
+          </cell>
+          <cell r="C77">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78">
+            <v>7700</v>
+          </cell>
+          <cell r="C78">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79">
+            <v>7800</v>
+          </cell>
+          <cell r="C79">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80">
+            <v>7900</v>
+          </cell>
+          <cell r="C80">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81">
+            <v>8000</v>
+          </cell>
+          <cell r="C81">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82">
+            <v>8100</v>
+          </cell>
+          <cell r="C82">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83">
+            <v>8200</v>
+          </cell>
+          <cell r="C83">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84">
+            <v>8300</v>
+          </cell>
+          <cell r="C84">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85">
+            <v>8400</v>
+          </cell>
+          <cell r="C85">
+            <v>75</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86">
+            <v>8500</v>
+          </cell>
+          <cell r="C86">
+            <v>20</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87">
+            <v>8600</v>
+          </cell>
+          <cell r="C87">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88">
+            <v>8700</v>
+          </cell>
+          <cell r="C88">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89">
+            <v>8800</v>
+          </cell>
+          <cell r="C89">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90">
+            <v>8900</v>
+          </cell>
+          <cell r="C90">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91">
+            <v>9000</v>
+          </cell>
+          <cell r="C91">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92">
+            <v>9100</v>
+          </cell>
+          <cell r="C92">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93">
+            <v>9200</v>
+          </cell>
+          <cell r="C93">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94">
+            <v>9300</v>
+          </cell>
+          <cell r="C94">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95">
+            <v>9400</v>
+          </cell>
+          <cell r="C95">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96">
+            <v>9500</v>
+          </cell>
+          <cell r="C96">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97">
+            <v>9600</v>
+          </cell>
+          <cell r="C97">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98">
+            <v>9700</v>
+          </cell>
+          <cell r="C98">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99">
+            <v>9800</v>
+          </cell>
+          <cell r="C99">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100">
+            <v>9900</v>
+          </cell>
+          <cell r="C100">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101">
+            <v>10000</v>
+          </cell>
+          <cell r="C101">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1355,7 +4192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -1892,4 +4729,1745 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>200</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>300</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>400</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>500</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>600</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>700</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>800</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>900</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1000</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1100</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1200</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1300</v>
+      </c>
+      <c r="B14">
+        <v>47</v>
+      </c>
+      <c r="C14">
+        <v>35</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1400</v>
+      </c>
+      <c r="B15">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1500</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1600</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1700</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1800</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1900</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2000</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2100</v>
+      </c>
+      <c r="B22">
+        <v>107</v>
+      </c>
+      <c r="C22">
+        <v>75</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2200</v>
+      </c>
+      <c r="B23">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>75</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2300</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2400</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2500</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2600</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2700</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2800</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2900</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3000</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>25</v>
+      </c>
+      <c r="E31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3100</v>
+      </c>
+      <c r="B32">
+        <v>107</v>
+      </c>
+      <c r="C32">
+        <v>75</v>
+      </c>
+      <c r="D32">
+        <v>91</v>
+      </c>
+      <c r="E32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3200</v>
+      </c>
+      <c r="B33">
+        <v>28</v>
+      </c>
+      <c r="C33">
+        <v>20</v>
+      </c>
+      <c r="D33">
+        <v>28</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3300</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>12</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3400</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3500</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3600</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3700</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3800</v>
+      </c>
+      <c r="B39">
+        <v>37</v>
+      </c>
+      <c r="C39">
+        <v>25</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3900</v>
+      </c>
+      <c r="B40">
+        <v>98</v>
+      </c>
+      <c r="C40">
+        <v>70</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>4000</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>4100</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>4200</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>4300</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>4400</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>4500</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>4600</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>8</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>4700</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>4800</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>4900</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>5000</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>35</v>
+      </c>
+      <c r="E51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>5100</v>
+      </c>
+      <c r="B52">
+        <v>37</v>
+      </c>
+      <c r="C52">
+        <v>25</v>
+      </c>
+      <c r="D52">
+        <v>69</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>5200</v>
+      </c>
+      <c r="B53">
+        <v>88</v>
+      </c>
+      <c r="C53">
+        <v>70</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>5300</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>12</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>5400</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>5500</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>5600</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>5700</v>
+      </c>
+      <c r="B58">
+        <v>12</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>5800</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>5900</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>6000</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>6100</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>6200</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>6300</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>6400</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>6500</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>6600</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>6700</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>6800</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>6900</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>7000</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>7100</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>7200</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>7300</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>8</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>7400</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>7500</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>7600</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>7700</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>35</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>7800</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>20</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>7900</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>8000</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>8100</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>8200</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>8</v>
+      </c>
+      <c r="E83">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>8300</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>8400</v>
+      </c>
+      <c r="B85">
+        <v>107</v>
+      </c>
+      <c r="C85">
+        <v>75</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>8500</v>
+      </c>
+      <c r="B86">
+        <v>28</v>
+      </c>
+      <c r="C86">
+        <v>20</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>8600</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>75</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>8700</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>20</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>8800</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>8900</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>9000</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>9100</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>9200</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>9300</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>9400</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>9500</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>8</v>
+      </c>
+      <c r="E96">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>9600</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>9700</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>9800</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>9900</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>75</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>10000</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>20</v>
+      </c>
+      <c r="E101">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>